<commit_message>
Kobla sammen to produkt som var feilaktig separert
</commit_message>
<xml_diff>
--- a/src/test/resources/substituttlister/V5_stoler_med_oppreisingsfunksjon.xlsx
+++ b/src/test/resources/substituttlister/V5_stoler_med_oppreisingsfunksjon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://navno-my.sharepoint.com/personal/kari_ihle_nav_no/Documents/Chatfiler for Microsoft Teams/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasmund/dev/hm-grunndata-alternativprodukter/src/test/resources/substituttlister/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56E20FD5-A619-4E6A-A529-82F202C3E655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70DDEE6-DABF-5D45-896A-54F9817AAB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="255" windowWidth="16590" windowHeight="15015" firstSheet="1" activeTab="1" xr2:uid="{DAB7D3D8-04D0-4DD5-9B74-78B882D95CED}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="16600" windowHeight="15020" firstSheet="1" activeTab="1" xr2:uid="{DAB7D3D8-04D0-4DD5-9B74-78B882D95CED}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -1419,7 +1419,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2536,7 +2536,7 @@
       <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2545,22 +2545,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3485A8-7267-48FD-BE99-693AE922852B}">
-  <dimension ref="A1:E266"/>
+  <dimension ref="A1:E265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A253" sqref="A253:XFD253"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="24" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="24" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2577,13 +2577,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="23"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="54">
+    <row r="3" spans="1:5" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>1</v>
       </c>
@@ -2594,7 +2594,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="27" t="s">
         <v>6</v>
@@ -2606,7 +2606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="27" t="s">
         <v>8</v>
@@ -2618,7 +2618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="27" t="s">
         <v>8</v>
@@ -2630,7 +2630,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="27" t="s">
         <v>11</v>
@@ -2642,13 +2642,13 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="23"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="27" t="s">
         <v>13</v>
@@ -2660,7 +2660,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="27" t="s">
         <v>15</v>
@@ -2672,7 +2672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="27" t="s">
         <v>17</v>
@@ -2684,7 +2684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="27" t="s">
         <v>19</v>
@@ -2696,7 +2696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="27" t="s">
         <v>19</v>
@@ -2708,13 +2708,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="23"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="27" t="s">
         <v>22</v>
@@ -2726,7 +2726,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="27" t="s">
         <v>23</v>
@@ -2738,7 +2738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="27" t="s">
         <v>23</v>
@@ -2750,13 +2750,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="23"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="27" t="s">
         <v>24</v>
@@ -2768,7 +2768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
       <c r="C20" s="27" t="s">
         <v>25</v>
@@ -2780,7 +2780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="27" t="s">
         <v>25</v>
@@ -2792,13 +2792,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="23"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="27" t="s">
         <v>26</v>
@@ -2810,7 +2810,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="27" t="s">
         <v>27</v>
@@ -2822,7 +2822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="27" t="s">
         <v>27</v>
@@ -2834,7 +2834,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
       <c r="C26" s="27" t="s">
         <v>29</v>
@@ -2846,7 +2846,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="27" t="s">
         <v>29</v>
@@ -2858,13 +2858,13 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="23"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="27" t="s">
         <v>32</v>
@@ -2876,7 +2876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="27" t="s">
         <v>33</v>
@@ -2886,7 +2886,7 @@
       </c>
       <c r="E30" s="29"/>
     </row>
-    <row r="31" spans="2:5">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="27" t="s">
         <v>33</v>
@@ -2898,7 +2898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="1"/>
       <c r="C32" s="27" t="s">
         <v>34</v>
@@ -2910,7 +2910,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="27" t="s">
         <v>34</v>
@@ -2922,13 +2922,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="23"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="27" t="s">
         <v>37</v>
@@ -2940,7 +2940,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="27" t="s">
         <v>38</v>
@@ -2952,7 +2952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="27" t="s">
         <v>38</v>
@@ -2964,7 +2964,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="27" t="s">
         <v>39</v>
@@ -2976,13 +2976,13 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="23"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="C40" s="27" t="s">
         <v>41</v>
@@ -2994,7 +2994,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="27" t="s">
         <v>42</v>
@@ -3006,7 +3006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="1"/>
       <c r="C42" s="27" t="s">
         <v>42</v>
@@ -3018,7 +3018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="27" t="s">
         <v>43</v>
@@ -3030,13 +3030,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="27"/>
       <c r="D44" s="28"/>
       <c r="E44" s="27"/>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="1"/>
       <c r="C45" s="27" t="s">
         <v>45</v>
@@ -3046,1529 +3046,1523 @@
       </c>
       <c r="E45" s="27"/>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="28"/>
+      <c r="C46" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" s="28">
+        <v>240520</v>
+      </c>
       <c r="E46" s="27"/>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
-      <c r="C47" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="D47" s="28">
-        <v>240520</v>
-      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="28"/>
       <c r="E47" s="27"/>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="1"/>
       <c r="C48" s="27"/>
       <c r="D48" s="28"/>
       <c r="E48" s="27"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B49" s="1"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="27"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="52" spans="1:5" ht="72">
-      <c r="A52" s="32">
+      <c r="C49" s="1"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="51" spans="1:5" ht="57" x14ac:dyDescent="0.3">
+      <c r="A51" s="32">
         <v>2</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B51" s="21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
-      <c r="B53" s="1" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="22">
+        <v>296140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D53" s="22">
-        <v>296140</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>240534</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D54" s="22">
-        <v>240534</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="C55" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D55" s="22">
         <v>195627</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
-      <c r="D56" s="22"/>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="B58" s="1" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D55" s="22"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="C57" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="22">
+        <v>296141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D58" s="22">
-        <v>296141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>240533</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C59" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D59" s="22">
-        <v>240533</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="C60" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D60" s="22">
         <v>195626</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
-      <c r="D61" s="22"/>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="B63" s="1" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D60" s="22"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C62" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D62" s="22">
+        <v>296142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C63" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D63" s="22">
-        <v>296142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>296310</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C64" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D64" s="22">
+        <v>296312</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C65" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" s="22">
+        <v>295771</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C66" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66" s="22">
+        <v>295772</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C67" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D67" s="22">
+        <v>240536</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C68" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D68" s="22">
+        <v>195735</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C69" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D69" s="22">
+        <v>195733</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D70" s="22"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D72" s="22">
+        <v>296143</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C73" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" s="22">
+        <v>296311</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C74" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D74" s="22">
+        <v>296313</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C75" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D75" s="22">
+        <v>295766</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C76" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D76" s="22">
+        <v>295767</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C77" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D77" s="22">
+        <v>240535</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C78" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" s="22">
+        <v>195734</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C79" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D79" s="22">
+        <v>195732</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D80" s="22"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B82" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D82" s="22">
+        <v>296144</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C83" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D64" s="22">
+      <c r="D83" s="22">
         <v>296310</v>
       </c>
     </row>
-    <row r="65" spans="2:4">
-      <c r="C65" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D65" s="22">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C84" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D84" s="22">
         <v>296312</v>
       </c>
     </row>
-    <row r="66" spans="2:4">
-      <c r="C66" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D66" s="22">
-        <v>295771</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4">
-      <c r="C67" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D67" s="22">
-        <v>295772</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4">
-      <c r="C68" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D68" s="22">
-        <v>240536</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4">
-      <c r="C69" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="22">
-        <v>195735</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4">
-      <c r="C70" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D70" s="22">
-        <v>195733</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4">
-      <c r="D71" s="22"/>
-    </row>
-    <row r="73" spans="2:4">
-      <c r="B73" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D73" s="22">
-        <v>296143</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4">
-      <c r="C74" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D74" s="22">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C85" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D85" s="22">
+        <v>295773</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C86" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D86" s="22">
+        <v>295774</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C87" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D87" s="22">
+        <v>240538</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C88" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D88" s="22">
+        <v>195625</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C89" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" s="22">
+        <v>195633</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C90" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D90" s="22">
+        <v>195739</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C91" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D91" s="22">
+        <v>195737</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B94" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D94" s="22">
+        <v>296145</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C95" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D95" s="22">
         <v>296311</v>
       </c>
     </row>
-    <row r="75" spans="2:4">
-      <c r="C75" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D75" s="22">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C96" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D96" s="22">
         <v>296313</v>
       </c>
     </row>
-    <row r="76" spans="2:4">
-      <c r="C76" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D76" s="22">
-        <v>295766</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4">
-      <c r="C77" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D77" s="22">
-        <v>295767</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4">
-      <c r="C78" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D78" s="22">
-        <v>240535</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4">
-      <c r="C79" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D79" s="22">
-        <v>195734</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4">
-      <c r="C80" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D80" s="22">
-        <v>195732</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5">
-      <c r="D81" s="22"/>
-    </row>
-    <row r="83" spans="2:5">
-      <c r="B83" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D83" s="22">
-        <v>296144</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5">
-      <c r="C84" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D84" s="22">
-        <v>296310</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5">
-      <c r="C85" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D85" s="22">
-        <v>296312</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5">
-      <c r="C86" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D86" s="22">
-        <v>295773</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5">
-      <c r="C87" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D87" s="22">
-        <v>295774</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5">
-      <c r="C88" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D88" s="22">
-        <v>240538</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5">
-      <c r="C89" s="2" t="s">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C97" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D97" s="22">
+        <v>295768</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C98" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D98" s="22">
+        <v>295769</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C99" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D99" s="22">
+        <v>240537</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C100" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D100" s="22">
+        <v>195624</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C101" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D101" s="22">
+        <v>195632</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C102" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D102" s="22">
+        <v>195738</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C103" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D103" s="22">
+        <v>195736</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D104" s="22"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B106" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D106" s="22">
+        <v>296146</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C107" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D107" s="22">
+        <v>296306</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C108" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D108" s="22">
+        <v>296308</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C109" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D109" s="22">
+        <v>296314</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C110" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D110" s="22">
+        <v>295775</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C111" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D111" s="22">
+        <v>240540</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C112" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D89" s="22">
+      <c r="D112" s="22">
         <v>195625</v>
       </c>
     </row>
-    <row r="90" spans="2:5">
-      <c r="C90" s="2" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C113" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D90" s="22">
+      <c r="D113" s="22">
         <v>195633</v>
       </c>
     </row>
-    <row r="91" spans="2:5">
-      <c r="C91" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D91" s="22">
-        <v>195739</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5">
-      <c r="C92" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D92" s="22">
-        <v>195737</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5">
-      <c r="D93" s="22"/>
-      <c r="E93" s="22"/>
-    </row>
-    <row r="95" spans="2:5">
-      <c r="B95" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D95" s="22">
-        <v>296145</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5">
-      <c r="C96" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D96" s="22">
-        <v>296311</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4">
-      <c r="C97" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D97" s="22">
-        <v>296313</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4">
-      <c r="C98" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D98" s="22">
-        <v>295768</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4">
-      <c r="C99" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D99" s="22">
-        <v>295769</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4">
-      <c r="C100" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D100" s="22">
-        <v>240537</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4">
-      <c r="C101" s="2" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C114" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D114" s="22">
+        <v>195741</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D115" s="22"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D116" s="22"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B117" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D117" s="22">
+        <v>296147</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C118" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D118" s="22">
+        <v>296307</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C119" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D119" s="22">
+        <v>296309</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C120" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D120" s="22">
+        <v>296315</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C121" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D121" s="22">
+        <v>295770</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C122" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D122" s="22">
+        <v>240539</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C123" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D101" s="22">
+      <c r="D123" s="22">
         <v>195624</v>
       </c>
     </row>
-    <row r="102" spans="2:4">
-      <c r="C102" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D102" s="22">
-        <v>195632</v>
-      </c>
-    </row>
-    <row r="103" spans="2:4">
-      <c r="C103" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D103" s="22">
-        <v>195738</v>
-      </c>
-    </row>
-    <row r="104" spans="2:4">
-      <c r="C104" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D104" s="22">
-        <v>195736</v>
-      </c>
-    </row>
-    <row r="105" spans="2:4">
-      <c r="D105" s="22"/>
-    </row>
-    <row r="107" spans="2:4">
-      <c r="B107" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D107" s="22">
-        <v>296146</v>
-      </c>
-    </row>
-    <row r="108" spans="2:4">
-      <c r="C108" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D108" s="22">
-        <v>296306</v>
-      </c>
-    </row>
-    <row r="109" spans="2:4">
-      <c r="C109" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D109" s="22">
-        <v>296308</v>
-      </c>
-    </row>
-    <row r="110" spans="2:4">
-      <c r="C110" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D110" s="22">
-        <v>296314</v>
-      </c>
-    </row>
-    <row r="111" spans="2:4">
-      <c r="C111" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D111" s="22">
-        <v>295775</v>
-      </c>
-    </row>
-    <row r="112" spans="2:4">
-      <c r="C112" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D112" s="22">
-        <v>240540</v>
-      </c>
-    </row>
-    <row r="113" spans="2:4">
-      <c r="C113" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D113" s="22">
-        <v>195625</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4">
-      <c r="C114" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D114" s="22">
-        <v>195633</v>
-      </c>
-    </row>
-    <row r="115" spans="2:4">
-      <c r="C115" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D115" s="22">
-        <v>195741</v>
-      </c>
-    </row>
-    <row r="116" spans="2:4">
-      <c r="D116" s="22"/>
-    </row>
-    <row r="117" spans="2:4">
-      <c r="D117" s="22"/>
-    </row>
-    <row r="118" spans="2:4">
-      <c r="B118" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D118" s="22">
-        <v>296147</v>
-      </c>
-    </row>
-    <row r="119" spans="2:4">
-      <c r="C119" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D119" s="22">
-        <v>296307</v>
-      </c>
-    </row>
-    <row r="120" spans="2:4">
-      <c r="C120" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D120" s="22">
-        <v>296309</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4">
-      <c r="C121" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D121" s="22">
-        <v>296315</v>
-      </c>
-    </row>
-    <row r="122" spans="2:4">
-      <c r="C122" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D122" s="22">
-        <v>295770</v>
-      </c>
-    </row>
-    <row r="123" spans="2:4">
-      <c r="C123" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D123" s="22">
-        <v>240539</v>
-      </c>
-    </row>
-    <row r="124" spans="2:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C124" s="2" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="D124" s="22">
-        <v>195624</v>
-      </c>
-    </row>
-    <row r="125" spans="2:4">
-      <c r="C125" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D125" s="22">
         <v>195740</v>
       </c>
     </row>
-    <row r="126" spans="2:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D125" s="22"/>
+    </row>
+    <row r="126" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D126" s="22"/>
     </row>
-    <row r="127" spans="2:4" ht="16.5" customHeight="1">
-      <c r="D127" s="22"/>
-    </row>
-    <row r="129" spans="1:4" ht="72">
-      <c r="A129" s="32">
+    <row r="128" spans="1:4" ht="76" x14ac:dyDescent="0.3">
+      <c r="A128" s="32">
         <v>3</v>
       </c>
-      <c r="B129" s="21" t="s">
+      <c r="B128" s="21" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
-      <c r="B130" s="2" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B129" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="C129" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D129" s="22">
+        <v>296148</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C130" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D130" s="22">
-        <v>296148</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4">
+        <v>295777</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C131" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D131" s="22">
-        <v>295777</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4">
+        <v>240522</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C132" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D132" s="22">
-        <v>240522</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4">
+        <v>195743</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C133" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D133" s="22">
+        <v>195637</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D134" s="22"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B136" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D136" s="22">
+        <v>296149</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C137" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D137" s="22">
+        <v>295776</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C138" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D138" s="22">
+        <v>240521</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C139" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D139" s="22">
+        <v>195742</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C140" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D140" s="22">
+        <v>195636</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="57" x14ac:dyDescent="0.3">
+      <c r="A144" s="32">
+        <v>4</v>
+      </c>
+      <c r="B144" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B145" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D145" s="22">
+        <v>296316</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C146" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D146" s="22">
+        <v>296318</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C147" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D147" s="22">
+        <v>296324</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C148" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D148" s="22">
+        <v>241480</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C149" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D149" s="22">
+        <v>241475</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C150" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D150" s="22">
+        <v>241460</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C151" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D151" s="22">
+        <v>241476</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C152" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D152" s="22">
+        <v>241478</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C153" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D153" s="22">
+        <v>241456</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C154" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D154" s="22">
+        <v>241458</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C155" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D155" s="22">
+        <v>296164</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C156" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D156" s="22">
+        <v>240550</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C157" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D157" s="22">
+        <v>240530</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C158" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D158" s="22">
+        <v>195742</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C159" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D159" s="22">
+        <v>195752</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B162" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D162" s="22">
+        <v>296162</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C163" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D163" s="22">
+        <v>240548</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C164" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D164" s="22">
+        <v>240528</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C165" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D165" s="22">
+        <v>195744</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C166" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D166" s="22">
+        <v>195750</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C167" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D167" s="22">
+        <v>195760</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C168" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D168" s="22">
+        <v>296320</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C169" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D169" s="22">
+        <v>296322</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C170" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D170" s="22">
+        <v>241484</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C171" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D171" s="22">
+        <v>241482</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C172" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D172" s="22">
+        <v>241464</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C173" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D173" s="22">
+        <v>241462</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B176" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D176" s="22">
+        <v>240544</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C177" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D177" s="22">
+        <v>240524</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C178" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D178" s="22">
+        <v>296158</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B181" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D181" s="22">
+        <v>296160</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C182" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D182" s="22">
+        <v>240546</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C183" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D183" s="22">
+        <v>195746</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C184" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D184" s="22">
+        <v>195748</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C185" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D185" s="22">
+        <v>195756</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C186" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D186" s="22">
+        <v>195758</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C187" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D187" s="22">
+        <v>195757</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B189" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D189" s="22">
+        <v>296317</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C190" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D190" s="22">
+        <v>296319</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C191" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D191" s="22">
+        <v>296325</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C192" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D192" s="22">
+        <v>296165</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C193" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D193" s="22">
+        <v>241479</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C194" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D194" s="22">
+        <v>241477</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C195" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D195" s="22">
+        <v>241459</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C196" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D196" s="22">
+        <v>241455</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C197" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D197" s="22">
+        <v>241457</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C198" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D198" s="22">
+        <v>240549</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C199" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D199" s="22">
+        <v>240529</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C200" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D200" s="22">
         <v>195743</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
-      <c r="C134" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D134" s="22">
-        <v>195637</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="D135" s="22"/>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="B137" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D137" s="22">
-        <v>296149</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="C138" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D138" s="22">
-        <v>295776</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="C139" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D139" s="22">
-        <v>240521</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="C140" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D140" s="22">
-        <v>195742</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="C141" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D141" s="22">
-        <v>195636</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="72">
-      <c r="A145" s="32">
-        <v>4</v>
-      </c>
-      <c r="B145" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4">
-      <c r="B146" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D146" s="22">
-        <v>296316</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4">
-      <c r="C147" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D147" s="22">
-        <v>296318</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4">
-      <c r="C148" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D148" s="22">
-        <v>296324</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4">
-      <c r="C149" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D149" s="22">
-        <v>241480</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4">
-      <c r="C150" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D150" s="22">
-        <v>241475</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4">
-      <c r="C151" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D151" s="22">
-        <v>241460</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4">
-      <c r="C152" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D152" s="22">
-        <v>241476</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4">
-      <c r="C153" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D153" s="22">
-        <v>241478</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4">
-      <c r="C154" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D154" s="22">
-        <v>241456</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4">
-      <c r="C155" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D155" s="22">
-        <v>241458</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4">
-      <c r="C156" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D156" s="22">
-        <v>296164</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4">
-      <c r="C157" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D157" s="22">
-        <v>240550</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4">
-      <c r="C158" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D158" s="22">
-        <v>240530</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4">
-      <c r="C159" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D159" s="22">
-        <v>195742</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4">
-      <c r="C160" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D160" s="22">
-        <v>195752</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4">
-      <c r="B163" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D163" s="22">
-        <v>296162</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4">
-      <c r="C164" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D164" s="22">
-        <v>240548</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4">
-      <c r="C165" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D165" s="22">
-        <v>240528</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4">
-      <c r="C166" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D166" s="22">
-        <v>195744</v>
-      </c>
-    </row>
-    <row r="167" spans="2:4">
-      <c r="C167" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D167" s="22">
-        <v>195750</v>
-      </c>
-    </row>
-    <row r="168" spans="2:4">
-      <c r="C168" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D168" s="22">
-        <v>195760</v>
-      </c>
-    </row>
-    <row r="169" spans="2:4">
-      <c r="C169" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D169" s="22">
-        <v>296320</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4">
-      <c r="C170" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D170" s="22">
-        <v>296322</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4">
-      <c r="C171" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D171" s="22">
-        <v>241484</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4">
-      <c r="C172" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D172" s="22">
-        <v>241482</v>
-      </c>
-    </row>
-    <row r="173" spans="2:4">
-      <c r="C173" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D173" s="22">
-        <v>241464</v>
-      </c>
-    </row>
-    <row r="174" spans="2:4">
-      <c r="C174" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D174" s="22">
-        <v>241462</v>
-      </c>
-    </row>
-    <row r="177" spans="2:4">
-      <c r="B177" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D177" s="22">
-        <v>240544</v>
-      </c>
-    </row>
-    <row r="178" spans="2:4">
-      <c r="C178" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D178" s="22">
-        <v>240524</v>
-      </c>
-    </row>
-    <row r="179" spans="2:4">
-      <c r="C179" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D179" s="22">
-        <v>296158</v>
-      </c>
-    </row>
-    <row r="182" spans="2:4">
-      <c r="B182" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D182" s="22">
-        <v>296160</v>
-      </c>
-    </row>
-    <row r="183" spans="2:4">
-      <c r="C183" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D183" s="22">
-        <v>240546</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4">
-      <c r="C184" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="D184" s="22">
-        <v>195746</v>
-      </c>
-    </row>
-    <row r="185" spans="2:4">
-      <c r="C185" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D185" s="22">
-        <v>195748</v>
-      </c>
-    </row>
-    <row r="186" spans="2:4">
-      <c r="C186" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D186" s="22">
-        <v>195756</v>
-      </c>
-    </row>
-    <row r="187" spans="2:4">
-      <c r="C187" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D187" s="22">
-        <v>195758</v>
-      </c>
-    </row>
-    <row r="188" spans="2:4">
-      <c r="C188" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D188" s="22">
-        <v>195757</v>
-      </c>
-    </row>
-    <row r="190" spans="2:4">
-      <c r="B190" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D190" s="22">
-        <v>296317</v>
-      </c>
-    </row>
-    <row r="191" spans="2:4">
-      <c r="C191" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D191" s="22">
-        <v>296319</v>
-      </c>
-    </row>
-    <row r="192" spans="2:4">
-      <c r="C192" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D192" s="22">
-        <v>296325</v>
-      </c>
-    </row>
-    <row r="193" spans="2:4">
-      <c r="C193" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D193" s="22">
-        <v>296165</v>
-      </c>
-    </row>
-    <row r="194" spans="2:4">
-      <c r="C194" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D194" s="22">
-        <v>241479</v>
-      </c>
-    </row>
-    <row r="195" spans="2:4">
-      <c r="C195" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D195" s="22">
-        <v>241477</v>
-      </c>
-    </row>
-    <row r="196" spans="2:4">
-      <c r="C196" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D196" s="22">
-        <v>241459</v>
-      </c>
-    </row>
-    <row r="197" spans="2:4">
-      <c r="C197" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D197" s="22">
-        <v>241455</v>
-      </c>
-    </row>
-    <row r="198" spans="2:4">
-      <c r="C198" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D198" s="22">
-        <v>241457</v>
-      </c>
-    </row>
-    <row r="199" spans="2:4">
-      <c r="C199" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D199" s="22">
-        <v>240549</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4">
-      <c r="C200" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D200" s="22">
-        <v>240529</v>
-      </c>
-    </row>
-    <row r="201" spans="2:4">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C201" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D201" s="22">
-        <v>195743</v>
-      </c>
-    </row>
-    <row r="202" spans="2:4">
+        <v>195753</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C202" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D202" s="22">
-        <v>195753</v>
-      </c>
-    </row>
-    <row r="203" spans="2:4">
-      <c r="C203" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D203" s="22">
         <v>195761</v>
       </c>
     </row>
-    <row r="206" spans="2:4">
-      <c r="B206" s="2" t="s">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B205" s="2" t="s">
         <v>179</v>
       </c>
+      <c r="C205" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D205" s="22">
+        <v>296321</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C206" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D206" s="22">
-        <v>296321</v>
-      </c>
-    </row>
-    <row r="207" spans="2:4">
+        <v>296323</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C207" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D207" s="22">
-        <v>296323</v>
-      </c>
-    </row>
-    <row r="208" spans="2:4">
+        <v>241483</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C208" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D208" s="22">
-        <v>241483</v>
-      </c>
-    </row>
-    <row r="209" spans="2:4">
+        <v>241481</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C209" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D209" s="22">
-        <v>241481</v>
-      </c>
-    </row>
-    <row r="210" spans="2:4">
+        <v>241463</v>
+      </c>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C210" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D210" s="22">
-        <v>241463</v>
-      </c>
-    </row>
-    <row r="211" spans="2:4">
+        <v>241461</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C211" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D211" s="22">
-        <v>241461</v>
-      </c>
-    </row>
-    <row r="212" spans="2:4">
+        <v>296163</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C212" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D212" s="22">
-        <v>296163</v>
-      </c>
-    </row>
-    <row r="213" spans="2:4">
+        <v>240547</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C213" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D213" s="22">
-        <v>240547</v>
-      </c>
-    </row>
-    <row r="214" spans="2:4">
+        <v>240527</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C214" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D214" s="22">
-        <v>240527</v>
-      </c>
-    </row>
-    <row r="215" spans="2:4">
+        <v>195745</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C215" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D215" s="22">
-        <v>195745</v>
-      </c>
-    </row>
-    <row r="216" spans="2:4">
+        <v>195755</v>
+      </c>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C216" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D216" s="22">
-        <v>195755</v>
-      </c>
-    </row>
-    <row r="217" spans="2:4">
-      <c r="C217" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D217" s="22">
         <v>195751</v>
       </c>
     </row>
-    <row r="218" spans="2:4">
-      <c r="D218" s="22"/>
-    </row>
-    <row r="219" spans="2:4">
-      <c r="B219" s="1" t="s">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D217" s="22"/>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B218" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="C218" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D218" s="22">
+        <v>296159</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C219" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D219" s="22">
-        <v>296159</v>
-      </c>
-    </row>
-    <row r="220" spans="2:4">
+        <v>240523</v>
+      </c>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C220" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D220" s="22">
-        <v>240523</v>
-      </c>
-    </row>
-    <row r="221" spans="2:4">
-      <c r="C221" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D221" s="22">
         <v>240543</v>
       </c>
     </row>
-    <row r="223" spans="2:4">
-      <c r="B223" s="1" t="s">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B222" s="1" t="s">
         <v>196</v>
       </c>
+      <c r="C222" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D222" s="22">
+        <v>296161</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C223" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D223" s="22">
-        <v>296161</v>
-      </c>
-    </row>
-    <row r="224" spans="2:4">
+        <v>195747</v>
+      </c>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C224" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D224" s="22">
-        <v>195747</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4">
+        <v>195749</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C225" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D225" s="22">
-        <v>195749</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4">
-      <c r="C226" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D226" s="22">
         <v>195759</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="90">
-      <c r="A230" s="32">
+    <row r="229" spans="1:4" ht="76" x14ac:dyDescent="0.3">
+      <c r="A229" s="32">
         <v>5</v>
       </c>
-      <c r="B230" s="21" t="s">
+      <c r="B229" s="21" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="232" spans="1:4">
-      <c r="B232" s="2" t="s">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B231" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="C231" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D231" s="22">
+        <v>296166</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C232" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D232" s="22">
-        <v>296166</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4">
+        <v>295789</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C233" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D233" s="22">
-        <v>295789</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4">
+        <v>240552</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C234" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D234" s="22">
-        <v>240552</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4">
+        <v>241081</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C235" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D235" s="22">
-        <v>241081</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4">
+        <v>196200</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C236" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D236" s="22">
-        <v>196200</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4">
-      <c r="C237" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D237" s="22">
         <v>195762</v>
       </c>
     </row>
-    <row r="240" spans="1:4">
-      <c r="B240" s="2" t="s">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B239" s="2" t="s">
         <v>209</v>
       </c>
+      <c r="C239" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D239" s="22">
+        <v>296167</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C240" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D240" s="22">
-        <v>296167</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4">
+        <v>295788</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C241" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D241" s="22">
-        <v>295788</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4">
+        <v>240551</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C242" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D242" s="22">
-        <v>240551</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4">
+        <v>241080</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C243" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D243" s="22">
-        <v>241080</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4">
+        <v>214</v>
+      </c>
+      <c r="D243" s="26">
+        <v>196199</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C244" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D244" s="26">
-        <v>196199</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4">
-      <c r="C245" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D245" s="25">
+      <c r="D244" s="25">
         <v>195763</v>
       </c>
     </row>
-    <row r="246" spans="1:4">
-      <c r="D246" s="25"/>
-    </row>
-    <row r="247" spans="1:4">
-      <c r="B247" s="2" t="s">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D245" s="25"/>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B246" s="2" t="s">
         <v>216</v>
       </c>
+      <c r="C246" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D246" s="22">
+        <v>196820</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C247" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D247" s="22">
-        <v>196820</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4">
+        <v>251670</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C248" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D248" s="22">
-        <v>251670</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4">
-      <c r="C249" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D249" s="22">
         <v>215297</v>
       </c>
     </row>
-    <row r="251" spans="1:4">
-      <c r="B251" s="2" t="s">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B250" s="2" t="s">
         <v>220</v>
       </c>
+      <c r="C250" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D250" s="22">
+        <v>248794</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C251" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D251" s="22">
-        <v>248794</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4">
-      <c r="C252" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D252" s="22">
         <v>269870</v>
       </c>
     </row>
-    <row r="253" spans="1:4">
-      <c r="D253" s="22"/>
-    </row>
-    <row r="256" spans="1:4" ht="36">
-      <c r="A256" s="32">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D252" s="22"/>
+    </row>
+    <row r="255" spans="1:4" ht="38" x14ac:dyDescent="0.3">
+      <c r="A255" s="32">
         <v>6</v>
       </c>
-      <c r="B256" s="21" t="s">
+      <c r="B255" s="21" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="257" spans="3:5">
-      <c r="C257" s="30" t="s">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C256" s="30" t="s">
         <v>224</v>
       </c>
+      <c r="D256" s="28">
+        <v>296288</v>
+      </c>
+    </row>
+    <row r="257" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C257" s="27" t="s">
+        <v>225</v>
+      </c>
       <c r="D257" s="28">
-        <v>296288</v>
-      </c>
-    </row>
-    <row r="258" spans="3:5">
+        <v>296289</v>
+      </c>
+    </row>
+    <row r="258" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C258" s="27" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D258" s="28">
-        <v>296289</v>
-      </c>
-    </row>
-    <row r="259" spans="3:5">
-      <c r="C259" s="27" t="s">
-        <v>226</v>
-      </c>
-      <c r="D259" s="28">
         <v>296290</v>
       </c>
     </row>
-    <row r="261" spans="3:5">
+    <row r="260" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C260" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D260" s="28">
+        <v>296285</v>
+      </c>
+      <c r="E260" s="29"/>
+    </row>
+    <row r="261" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C261" s="27" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D261" s="28">
-        <v>296285</v>
-      </c>
-      <c r="E261" s="29"/>
-    </row>
-    <row r="262" spans="3:5">
+        <v>244819</v>
+      </c>
+      <c r="E261" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="262" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C262" s="27" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D262" s="28">
-        <v>244819</v>
-      </c>
-      <c r="E262" s="27" t="s">
+        <v>296286</v>
+      </c>
+      <c r="E262" s="29"/>
+    </row>
+    <row r="263" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C263" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="D263" s="28">
+        <v>239900</v>
+      </c>
+      <c r="E263" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="263" spans="3:5">
-      <c r="C263" s="27" t="s">
-        <v>229</v>
-      </c>
-      <c r="D263" s="28">
-        <v>296286</v>
-      </c>
-      <c r="E263" s="29"/>
-    </row>
-    <row r="264" spans="3:5">
+    <row r="264" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C264" s="27" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D264" s="28">
-        <v>239900</v>
-      </c>
-      <c r="E264" s="27" t="s">
+        <v>296287</v>
+      </c>
+      <c r="E264" s="29"/>
+    </row>
+    <row r="265" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C265" s="27" t="s">
+        <v>232</v>
+      </c>
+      <c r="D265" s="28">
+        <v>236421</v>
+      </c>
+      <c r="E265" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="265" spans="3:5">
-      <c r="C265" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="D265" s="28">
-        <v>296287</v>
-      </c>
-      <c r="E265" s="29"/>
-    </row>
-    <row r="266" spans="3:5">
-      <c r="C266" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="D266" s="28">
-        <v>236421</v>
-      </c>
-      <c r="E266" s="27" t="s">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D244">
+  <conditionalFormatting sqref="D243">
     <cfRule type="duplicateValues" dxfId="6" priority="1" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="5" priority="2" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="4" priority="3" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="3" priority="4" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D245:D246">
+  <conditionalFormatting sqref="D244:D245">
     <cfRule type="duplicateValues" dxfId="2" priority="8" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="1" priority="9" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="10" stopIfTrue="1"/>
@@ -4586,16 +4580,16 @@
       <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4612,7 +4606,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -4627,7 +4621,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="8" t="s">
@@ -4638,7 +4632,7 @@
       </c>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="8" t="s">
@@ -4649,7 +4643,7 @@
       </c>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="8" t="s">
@@ -4660,7 +4654,7 @@
       </c>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="8" t="s">
@@ -4671,7 +4665,7 @@
       </c>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="8" t="s">
@@ -4682,14 +4676,14 @@
       </c>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -4704,7 +4698,7 @@
       </c>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="8" t="s">
@@ -4715,14 +4709,14 @@
       </c>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>3</v>
       </c>
@@ -4737,7 +4731,7 @@
       </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="14" t="s">
@@ -4748,7 +4742,7 @@
       </c>
       <c r="E13" s="16"/>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="17" t="s">
@@ -4759,7 +4753,7 @@
       </c>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="17" t="s">
@@ -4770,7 +4764,7 @@
       </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="17" t="s">
@@ -4781,7 +4775,7 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="17" t="s">
@@ -4792,7 +4786,7 @@
       </c>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="17" t="s">
@@ -4803,7 +4797,7 @@
       </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:5" ht="30">
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="17" t="s">
@@ -4814,7 +4808,7 @@
       </c>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="17" t="s">
@@ -4825,7 +4819,7 @@
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="17" t="s">
@@ -4836,7 +4830,7 @@
       </c>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="17" t="s">
@@ -4847,7 +4841,7 @@
       </c>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="17" t="s">
@@ -4858,7 +4852,7 @@
       </c>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="17" t="s">
@@ -4869,7 +4863,7 @@
       </c>
       <c r="E24" s="12"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="17" t="s">
@@ -4880,14 +4874,14 @@
       </c>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="17"/>
       <c r="D26" s="9"/>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="1:5" ht="30">
+    <row r="27" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>4</v>
       </c>
@@ -4902,7 +4896,7 @@
       </c>
       <c r="E27" s="12"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="8" t="s">
@@ -4913,7 +4907,7 @@
       </c>
       <c r="E28" s="12"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="18"/>
       <c r="C29" s="8" t="s">
@@ -4924,14 +4918,14 @@
       </c>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="18"/>
       <c r="C30" s="8"/>
       <c r="D30" s="9"/>
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>5</v>
       </c>
@@ -4946,7 +4940,7 @@
       </c>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="11"/>
       <c r="C32" s="8" t="s">
@@ -4957,7 +4951,7 @@
       </c>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="18"/>
       <c r="C33" s="8" t="s">
@@ -4968,7 +4962,7 @@
       </c>
       <c r="E33" s="12"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="18"/>
       <c r="C34" s="8" t="s">
@@ -4979,7 +4973,7 @@
       </c>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="18"/>
       <c r="C35" s="8" t="s">
@@ -4990,7 +4984,7 @@
       </c>
       <c r="E35" s="12"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="18"/>
       <c r="C36" s="8" t="s">
@@ -5001,7 +4995,7 @@
       </c>
       <c r="E36" s="12"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="18"/>
       <c r="C37" s="8" t="s">
@@ -5012,7 +5006,7 @@
       </c>
       <c r="E37" s="12"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="18"/>
       <c r="C38" s="8" t="s">
@@ -5023,7 +5017,7 @@
       </c>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="18"/>
       <c r="C39" s="8" t="s">
@@ -5034,7 +5028,7 @@
       </c>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="18"/>
       <c r="C40" s="8" t="s">
@@ -5045,7 +5039,7 @@
       </c>
       <c r="E40" s="12"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="18"/>
       <c r="C41" s="8" t="s">
@@ -5056,7 +5050,7 @@
       </c>
       <c r="E41" s="12"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="18"/>
       <c r="C42" s="8" t="s">
@@ -5067,7 +5061,7 @@
       </c>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="18"/>
       <c r="C43" s="8" t="s">
@@ -5078,7 +5072,7 @@
       </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="18"/>
       <c r="C44" s="8" t="s">
@@ -5089,7 +5083,7 @@
       </c>
       <c r="E44" s="12"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="18"/>
       <c r="C45" s="8" t="s">
@@ -5100,7 +5094,7 @@
       </c>
       <c r="E45" s="12"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="18"/>
       <c r="C46" s="8" t="s">
@@ -5111,7 +5105,7 @@
       </c>
       <c r="E46" s="12"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="18"/>
       <c r="C47" s="8" t="s">
@@ -5122,7 +5116,7 @@
       </c>
       <c r="E47" s="12"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="18"/>
       <c r="C48" s="8" t="s">
@@ -5133,7 +5127,7 @@
       </c>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="18"/>
       <c r="C49" s="8" t="s">
@@ -5144,7 +5138,7 @@
       </c>
       <c r="E49" s="12"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="18"/>
       <c r="C50" s="8" t="s">
@@ -5155,7 +5149,7 @@
       </c>
       <c r="E50" s="12"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="18"/>
       <c r="C51" s="8" t="s">
@@ -5166,7 +5160,7 @@
       </c>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="18"/>
       <c r="C52" s="8" t="s">
@@ -5177,7 +5171,7 @@
       </c>
       <c r="E52" s="12"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="18"/>
       <c r="C53" s="8" t="s">
@@ -5188,7 +5182,7 @@
       </c>
       <c r="E53" s="12"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="18"/>
       <c r="C54" s="8" t="s">
@@ -5199,7 +5193,7 @@
       </c>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="18"/>
       <c r="C55" s="8" t="s">
@@ -5210,7 +5204,7 @@
       </c>
       <c r="E55" s="12"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="18"/>
       <c r="C56" s="8" t="s">
@@ -5221,7 +5215,7 @@
       </c>
       <c r="E56" s="12"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="18"/>
       <c r="C57" s="8" t="s">
@@ -5232,14 +5226,14 @@
       </c>
       <c r="E57" s="12"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="18"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
       <c r="E58" s="12"/>
     </row>
-    <row r="59" spans="1:5" ht="45">
+    <row r="59" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>6</v>
       </c>
@@ -5254,14 +5248,14 @@
       </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="18"/>
       <c r="C60" s="8"/>
       <c r="D60" s="9"/>
       <c r="E60" s="12"/>
     </row>
-    <row r="61" spans="1:5" ht="45">
+    <row r="61" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>7</v>
       </c>
@@ -5278,7 +5272,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3"/>
       <c r="B62" s="18"/>
       <c r="C62" s="8" t="s">
@@ -5289,7 +5283,7 @@
       </c>
       <c r="E62" s="20"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="18"/>
       <c r="C63" s="8" t="s">
@@ -5313,15 +5307,15 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5338,7 +5332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>326</v>
       </c>
@@ -5353,7 +5347,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
@@ -5364,7 +5358,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
@@ -5375,14 +5369,14 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
@@ -5393,7 +5387,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
@@ -5404,7 +5398,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
@@ -5415,14 +5409,14 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
@@ -5433,7 +5427,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -5444,7 +5438,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -5455,35 +5449,35 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>

</xml_diff>